<commit_message>
First full working condition
</commit_message>
<xml_diff>
--- a/templates/timesheet_template.xlsx
+++ b/templates/timesheet_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernard\Dropbox\Personal\python\auto_timesheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernard\Dropbox\Personal\python\auto_timesheet\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0FBEE7-5D5D-4BE4-898F-5718820E750A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E533156-8F44-4B2D-BD79-5F365C04E861}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{040EAB7B-2414-4E70-9EA4-53E04FDAF18E}"/>
+    <workbookView xWindow="15375" yWindow="2625" windowWidth="12885" windowHeight="11505" xr2:uid="{040EAB7B-2414-4E70-9EA4-53E04FDAF18E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,45 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>office use</t>
-  </si>
-  <si>
-    <t>week 1</t>
-  </si>
-  <si>
-    <t>week 2</t>
-  </si>
-  <si>
-    <t>week 3</t>
-  </si>
-  <si>
-    <t>week 4</t>
-  </si>
-  <si>
-    <t>d1</t>
-  </si>
-  <si>
-    <t>d2</t>
-  </si>
-  <si>
-    <t>d3</t>
-  </si>
-  <si>
-    <t>d4</t>
-  </si>
-  <si>
-    <t>u1</t>
-  </si>
-  <si>
-    <t>u2</t>
-  </si>
-  <si>
-    <t>u3</t>
-  </si>
-  <si>
-    <t>u4</t>
   </si>
   <si>
     <t>timesheet</t>
@@ -452,7 +416,7 @@
   <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,79 +428,39 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-    </row>
+    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>